<commit_message>
Improve scenario navigation and response input
Update Streamlit app to manage scenario state, track scenario counts, and generate unique keys for text area inputs to prevent state loss across reruns.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 6f65efa8-20c1-44f7-b31a-a103fc080719
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f3a459c4-9f70-4415-90bd-0b64d7ace412/6f65efa8-20c1-44f7-b31a-a103fc080719/YbzRgsk
</commit_message>
<xml_diff>
--- a/Coach_Training_Scenarios_ICF_PCC.xlsx
+++ b/Coach_Training_Scenarios_ICF_PCC.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Career" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Leadership" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Relationship" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Self Improvement" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Value System" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Career" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Leadership" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Relationship" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Self Improvement" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Value System" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,58 +465,234 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>C001</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>I feel stuck in my current role. I've been doing the same thing for 5 years and I'm not sure if I should stay or look for something new.</t>
+          <t>I’ve been in my job for years and feel like I’m not growing anymore.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>What would feeling unstuck look like for you?</t>
+          <t>What does growth mean to you right now?</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>If you imagine yourself five years from now, what does success look like?</t>
+          <t>What would it look like if you were fulfilled at work?</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>What's the cost of staying versus the cost of leaving?</t>
+          <t>What part of you is asking for change?</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>C002</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>I got passed over for a promotion again. My manager says I need to be more strategic, but I don't know what that means.</t>
+          <t>I keep getting overlooked for promotions and it’s starting to affect my confidence.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>What does 'being strategic' mean to you?</t>
+          <t>How do you interpret being overlooked?</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>When you think about leaders you admire, what behaviors do they demonstrate that you'd like to embody?</t>
+          <t>What story might you be telling yourself about this situation?</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>What would be different if you were showing up more strategically?</t>
-        </is>
-      </c>
+          <t>What kind of recognition feels meaningful to you?</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>I love my field but dread going to work most days.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>What’s missing that used to make it enjoyable?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>What might you be tolerating that drains your energy?</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>I’m torn between staying in a stable job and pursuing something uncertain that excites me.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>What does stability give you?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>What draws you to the uncertainty?</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>What would balance between the two look like?</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>I just got promoted and I feel like I don’t belong at this level.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>What does belonging mean to you here?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>How do you usually respond when you doubt yourself?</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>What helps you remember your capabilities?</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>I’m unsure if I picked the right career path at all.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>What drew you to it initially?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>What does a 'right path' look like for you?</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>If you could redesign it, what would be different?</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>I feel pressure to achieve more even though I’m already doing well.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Where does that pressure come from?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>How do you define 'enough' for yourself?</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>I struggle with setting boundaries at work without feeling guilty.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>What does saying 'no' represent for you?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>What might make boundary-setting feel safer?</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>I’m considering a career change but fear starting over.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>What part of starting over feels hardest?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>What possibilities come with a fresh start?</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>I can’t decide whether to take a job that pays more but feels misaligned with my values.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>What values would be honored or compromised?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>How might alignment and compensation coexist for you?</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -529,7 +705,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,58 +741,214 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>L001</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>My team doesn't seem motivated anymore. I try to be supportive, but nothing seems to work.</t>
+          <t>My team isn’t as motivated as I’d like them to be.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>What does motivation look like to you, and how would you know if your team had it?</t>
+          <t>What do you notice about their engagement?</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>What have you noticed about when your team is most engaged?</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>How might your own energy be influencing the team's motivation?</t>
-        </is>
-      </c>
+          <t>What might they be needing from your leadership?</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>L002</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>I have to give difficult feedback to a team member who's underperforming, but I'm worried about damaging our relationship.</t>
+          <t>I’m new in this leadership role and afraid of making mistakes.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>What's the relationship you want to have on the other side of this conversation?</t>
+          <t>What does making a mistake mean to you as a leader?</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>What might happen if you don't have this conversation?</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>How can you deliver this feedback in a way that honors both the relationship and the standards you hold?</t>
-        </is>
-      </c>
+          <t>What kind of leader do you want to be known as?</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>I find it hard to delegate — I end up doing most things myself.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>What makes delegation difficult for you?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>What could trusting others open up for you?</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>One of my team members constantly challenges me in meetings.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>What do you think they’re trying to communicate?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>What might this be offering you as a growth opportunity?</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>I want to inspire people, but I’m not sure how to connect emotionally with them.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>What does authentic connection look like to you?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>When have you felt inspired by someone — what did they do?</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>I’m struggling with imposter feelings even though I’m performing well.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>When did you first notice that feeling?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>What helps you recognize your strengths in these moments?</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>I avoid giving tough feedback because I don’t want to hurt anyone.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>What do you believe will happen if you give that feedback?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>How might feedback serve growth instead of harm?</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>I feel isolated at the top — I can’t share my doubts with anyone at work.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Who could be part of your support system?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>What would it mean to allow vulnerability in leadership?</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>My manager’s expectations seem unclear, and it’s causing stress.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>What clarity do you need most?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>How might you initiate that conversation?</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>I want to lead with empathy but still get results.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>How do you define empathy in leadership?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>What would balance look like between care and accountability?</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -629,7 +961,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -665,58 +997,214 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>R001</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>My partner and I keep having the same argument over and over. We just can't seem to communicate effectively.</t>
+          <t>I feel unheard in my relationship, like my partner doesn’t really get me.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>What pattern do you notice in how these arguments unfold?</t>
+          <t>What does being heard look like for you?</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>What would effective communication look like for you?</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>What's underneath this recurring argument for you?</t>
-        </is>
-      </c>
+          <t>How have you tried expressing this need before?</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>R002</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>I feel like I'm always the one making compromises in my relationships. How do I set better boundaries?</t>
+          <t>I avoid conflicts and end up suppressing how I really feel.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>What would honoring yourself fully look like in these relationships?</t>
+          <t>What happens for you when you avoid conflict?</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>What are you afraid might happen if you set that boundary?</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Where in your life are you already setting boundaries successfully?</t>
-        </is>
-      </c>
+          <t>What might be possible if you allowed your feelings to be seen?</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>I feel jealous even when I know I shouldn’t.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>What might jealousy be trying to tell you?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>How could you meet the need underneath it?</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>I love my partner but sometimes I crave more independence.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>What does independence mean to you in this context?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>How might you express that without creating distance?</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>I keep attracting the same type of partner and ending up disappointed.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>What patterns do you notice in these relationships?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>What part of you might be seeking familiarity?</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>I don’t know how to rebuild trust after being hurt.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>What would rebuilding trust look like for you?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>What does forgiveness mean in your situation?</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>I often feel responsible for my partner’s emotions.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>What makes you feel responsible for how they feel?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>What would it look like to let them hold their own emotions?</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>I’m afraid to be fully myself in my relationship.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>What part of yourself do you hold back?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>What would it take to bring more of you into the relationship?</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>I feel torn between family expectations and my partner’s needs.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>What values are in tension here?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>What would honoring both sides look like?</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>I’ve grown but my relationship hasn’t kept up.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>What do you need now that you didn’t before?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>What does growth mean for the two of you together?</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -729,7 +1217,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -765,58 +1253,214 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>S001</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>I know I should exercise and eat better, but I just can't seem to stick with it. I start strong and then give up.</t>
+          <t>I’m constantly overthinking every decision I make.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>What happens right before you give up?</t>
+          <t>What are you hoping to avoid by overthinking?</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>What would be different if this time you didn't give up?</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>What are you really committed to in your life right now?</t>
-        </is>
-      </c>
+          <t>What might trusting yourself look like?</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>S002</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>I'm a perfectionist and it's holding me back. I spend too much time on details and never feel like my work is good enough.</t>
+          <t>I struggle with self-discipline and often let myself down.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>What would 'good enough' look like?</t>
+          <t>What’s underneath that pattern?</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>What's the gift that your perfectionism has given you?</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>What becomes possible when you let go of perfect?</t>
-        </is>
-      </c>
+          <t>What helps you stay committed when you truly care?</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>I want to be more confident but don’t know where to start.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>What does confidence feel like to you?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>When have you felt confident before — what was different?</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>I’m afraid of being judged if I show the real me.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Who are you when you’re not managing others’ perceptions?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>What would acceptance look like if it started from within?</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>I procrastinate even when I know it’s hurting me.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>What’s the emotion behind your procrastination?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>What might progress, not perfection, look like?</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>I’m harsh on myself when I make mistakes.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>What would compassion sound like in those moments?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>What belief drives that self-talk?</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>I feel lost — like I don’t know who I am anymore.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>What parts of you feel forgotten or quiet lately?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>What might rediscovering yourself involve?</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>I can’t seem to sustain motivation for my goals.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>What’s missing that would make those goals meaningful again?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>How do you know when something truly matters to you?</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>I’m comparing myself to others all the time.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>What happens for you when you compare yourself?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>What might celebrating your own path look like?</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>I want to break free from old habits that don’t serve me anymore.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>What purpose did those habits once serve?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>What new pattern could replace them now?</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -829,7 +1473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -865,58 +1509,214 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>V001</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>I feel like I'm living someone else's life. I have a great job and family, but something feels off.</t>
+          <t>I’m not sure what my core values are anymore.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>What would living your own life look like?</t>
+          <t>What qualities feel most essential to who you are?</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>If you could design your life from scratch today, what would you keep and what would you change?</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>What values are you honoring, and which ones are you compromising?</t>
-        </is>
-      </c>
+          <t>When do you feel most aligned with yourself?</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>V002</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>I'm torn between taking a higher-paying job that requires more travel and staying in my current role where I can be home with my kids every night.</t>
+          <t>I feel torn between what I believe and what others expect of me.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>What matters most to you right now in this season of your life?</t>
+          <t>What’s the cost of betraying your own values?</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>How do you want to feel about this decision a year from now?</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>What would help you know you're making the right choice for you?</t>
-        </is>
-      </c>
+          <t>What would honoring them look like here?</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>I sometimes compromise my values to keep the peace.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>What value are you protecting when you do that?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>What would standing firm respectfully look like?</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>I want to live with more integrity but struggle with fear of judgment.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>What does integrity mean to you in daily life?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>What might courage look like in this context?</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>I feel disconnected from what truly matters to me.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>When was the last time you felt deeply connected?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>What helped you feel that way?</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>I’m chasing success but wonder if it aligns with who I want to be.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>How do you define success for yourself?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>What part of this pursuit feels off?</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>I want to make a difference but don’t know where to start.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>What kind of impact feels meaningful to you?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>What’s one small way to begin?</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>I’m facing a moral dilemma at work and it’s weighing on me.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>What values are in conflict here?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>What outcome would feel most aligned for you?</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>I’ve realized I’ve been living by others’ standards, not mine.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Whose standards have you been following?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>What does living by your own look like?</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>I’m questioning what legacy I want to leave behind.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>What would you want people to remember about you?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>How could you start embodying that today?</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>